<commit_message>
Ejercico a espera de repaso
</commit_message>
<xml_diff>
--- a/ReporteFinal.xlsx
+++ b/ReporteFinal.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <x:si>
     <x:t>Nombre Proyecto</x:t>
   </x:si>
@@ -35,6 +35,81 @@
   </x:si>
   <x:si>
     <x:t>24000.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AL071236</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AL112347</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AL213557</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AL221556</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AL232310</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AL258112</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AL258113</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AR044321</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AR056691</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15000.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AR062233</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AR062331</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UL046321</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17000.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UL054239</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UL223314</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UL258001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UL258122</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UL258129</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UR047451</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14166.67</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UR054912</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UR216878</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UR237511</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UR332441</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -423,6 +498,182 @@
         <x:v>6</x:v>
       </x:c>
     </x:row>
+    <x:row r="5" spans="1:2">
+      <x:c r="A5" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:2">
+      <x:c r="A6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:2">
+      <x:c r="A7" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:2">
+      <x:c r="A8" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:2">
+      <x:c r="A9" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:2">
+      <x:c r="A10" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:2">
+      <x:c r="A11" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:2">
+      <x:c r="A12" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:2">
+      <x:c r="A13" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:2">
+      <x:c r="A14" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:2">
+      <x:c r="A15" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:2">
+      <x:c r="A16" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:2">
+      <x:c r="A17" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:2">
+      <x:c r="A18" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:2">
+      <x:c r="A19" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:2">
+      <x:c r="A20" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:2">
+      <x:c r="A21" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:2">
+      <x:c r="A22" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:2">
+      <x:c r="A23" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:2">
+      <x:c r="A24" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:2">
+      <x:c r="A25" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:2">
+      <x:c r="A26" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>